<commit_message>
[Update] Ask Copilot to generate a clearner code, but still need to debug cause there are some wierd SPN label that get into the Excel file.
</commit_message>
<xml_diff>
--- a/Service_Watch_Test/Railblazer_Service watch data logger- Advancer-sDRC - 29th September 23.xlsx
+++ b/Service_Watch_Test/Railblazer_Service watch data logger- Advancer-sDRC - 29th September 23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tranetechnologies-my.sharepoint.com/personal/quant_vo_tranetechnologies_com/Documents/Documents/SysEng/Work/Standardize Service Watch Requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u245231\Quan_Vo\Local_Dev\complete-pandas-tutorial\Service_Watch_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{C125BCE7-8620-41B1-805A-2EC0AE24965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8ACCD6-6BDE-4F58-A88C-862AA0571073}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1403A3FA-1B65-4E68-A843-8F716135D860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ServiceWatch Log Parameters" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ServiceWatch Log Parameters'!$A$1:$O$131</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1441,9 +1441,6 @@
     <t xml:space="preserve">SPN Acronym </t>
   </si>
   <si>
-    <t xml:space="preserve">SPN </t>
-  </si>
-  <si>
     <t>Parameter Name (as read in SW data log)</t>
   </si>
   <si>
@@ -1898,6 +1895,9 @@
   <si>
     <t xml:space="preserve">P.Carr 29th September 23 - removing from list - not applicable for RB. 
 This is a Duplicate, already supported in this list in separate line item (refer to "temperature control mode", SPN 0x00F0). . </t>
+  </si>
+  <si>
+    <t>SPN</t>
   </si>
 </sst>
 </file>
@@ -2796,40 +2796,40 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="36" style="33" customWidth="1"/>
-    <col min="12" max="12" width="61.42578125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="111.85546875" customWidth="1"/>
+    <col min="12" max="12" width="61.44140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="111.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>376</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>377</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>378</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>0</v>
@@ -2859,27 +2859,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>360</v>
       </c>
       <c r="E2" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="F2" s="35" t="s">
         <v>420</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="G2" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="H2" s="31" t="b">
         <v>0</v>
@@ -2896,27 +2896,27 @@
       <c r="L2" s="14"/>
       <c r="M2"/>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>361</v>
       </c>
       <c r="E3" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>420</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="G3" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="H3" s="31" t="b">
         <v>0</v>
@@ -2933,27 +2933,27 @@
       <c r="L3" s="14"/>
       <c r="M3"/>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>362</v>
       </c>
       <c r="E4" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>420</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="G4" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="H4" s="31" t="b">
         <v>0</v>
@@ -2970,27 +2970,27 @@
       <c r="L4" s="14"/>
       <c r="M4"/>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>363</v>
       </c>
       <c r="E5" s="35" t="s">
+        <v>419</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>420</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="G5" s="31" t="s">
         <v>421</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>422</v>
       </c>
       <c r="H5" s="31" t="b">
         <v>0</v>
@@ -3007,12 +3007,12 @@
       <c r="L5" s="14"/>
       <c r="M5"/>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>176</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>177</v>
@@ -3039,22 +3039,22 @@
         <v>19</v>
       </c>
       <c r="K6" s="70" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L6" s="11"/>
       <c r="M6" s="77" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D7" s="85" t="s">
         <v>364</v>
@@ -3082,15 +3082,15 @@
       </c>
       <c r="L7" s="14"/>
       <c r="M7" s="80" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>262</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>263</v>
@@ -3117,19 +3117,19 @@
         <v>19</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="77" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>230</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>231</v>
@@ -3165,12 +3165,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>276</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>277</v>
@@ -3204,12 +3204,12 @@
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>280</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>281</v>
@@ -3240,12 +3240,12 @@
       </c>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>120</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>121</v>
@@ -3276,18 +3276,18 @@
       </c>
       <c r="L12" s="11"/>
     </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C13" s="41" t="s">
+        <v>478</v>
+      </c>
+      <c r="D13" s="41" t="s">
         <v>479</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>480</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>27</v>
@@ -3296,7 +3296,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H13" s="19" t="b">
         <v>1</v>
@@ -3313,18 +3313,18 @@
       <c r="L13" s="14"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
+        <v>481</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="C14" s="41" t="s">
         <v>482</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="C14" s="41" t="s">
+      <c r="D14" s="41" t="s">
         <v>483</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>484</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>27</v>
@@ -3333,7 +3333,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H14" s="19" t="b">
         <v>1</v>
@@ -3350,12 +3350,12 @@
       <c r="L14" s="14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>172</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>173</v>
@@ -3386,18 +3386,18 @@
       </c>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>27</v>
@@ -3423,12 +3423,12 @@
       <c r="L16" s="11"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>102</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>103</v>
@@ -3460,12 +3460,12 @@
       <c r="L17" s="11"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>79</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>80</v>
@@ -3496,18 +3496,18 @@
       </c>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>246</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>247</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>10</v>
@@ -3532,12 +3532,12 @@
       </c>
       <c r="L19" s="11"/>
     </row>
-    <row r="20" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
         <v>226</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C20" s="58" t="s">
         <v>227</v>
@@ -3570,15 +3570,15 @@
         <v>32</v>
       </c>
       <c r="M20" s="55" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>256</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>257</v>
@@ -3612,12 +3612,12 @@
       </c>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C22" s="58" t="s">
         <v>222</v>
@@ -3650,15 +3650,15 @@
         <v>225</v>
       </c>
       <c r="M22" s="55" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>241</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>242</v>
@@ -3691,12 +3691,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>201</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>202</v>
@@ -3730,15 +3730,15 @@
       </c>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D25" s="37" t="s">
         <v>365</v>
@@ -3750,7 +3750,7 @@
         <v>11</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H25" s="31" t="b">
         <v>1</v>
@@ -3762,20 +3762,20 @@
         <v>19</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L25" s="14"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D26" s="37" t="s">
         <v>366</v>
@@ -3787,7 +3787,7 @@
         <v>11</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H26" s="31" t="b">
         <v>1</v>
@@ -3799,17 +3799,17 @@
         <v>13</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L26" s="14"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>303</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>304</v>
@@ -3836,19 +3836,19 @@
         <v>19</v>
       </c>
       <c r="K27" s="70" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="77" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>66</v>
@@ -3875,19 +3875,19 @@
         <v>19</v>
       </c>
       <c r="K28" s="70" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="77" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>58</v>
@@ -3914,19 +3914,19 @@
         <v>19</v>
       </c>
       <c r="K29" s="70" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="77" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
         <v>248</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>249</v>
@@ -3959,12 +3959,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
         <v>185</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>186</v>
@@ -3991,19 +3991,19 @@
         <v>19</v>
       </c>
       <c r="K31" s="70" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L31" s="11"/>
       <c r="M31" s="55" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
         <v>197</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C32" s="58" t="s">
         <v>198</v>
@@ -4036,15 +4036,15 @@
         <v>200</v>
       </c>
       <c r="M32" s="55" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="56" t="s">
         <v>194</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C33" s="58" t="s">
         <v>195</v>
@@ -4077,15 +4077,15 @@
         <v>64</v>
       </c>
       <c r="M33" s="55" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="56" t="s">
         <v>188</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C34" s="58" t="s">
         <v>189</v>
@@ -4118,15 +4118,15 @@
         <v>64</v>
       </c>
       <c r="M34" s="55" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>191</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>192</v>
@@ -4156,12 +4156,12 @@
       <c r="L35" s="11"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>149</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>150</v>
@@ -4197,12 +4197,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>139</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>140</v>
@@ -4238,12 +4238,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>135</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>136</v>
@@ -4279,12 +4279,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>161</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>162</v>
@@ -4320,12 +4320,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>143</v>
@@ -4361,12 +4361,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>164</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>165</v>
@@ -4398,15 +4398,15 @@
       <c r="L41" s="11"/>
       <c r="M41"/>
     </row>
-    <row r="42" spans="1:13" s="7" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="7" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="75" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C42" s="73" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D42" s="73" t="s">
         <v>320</v>
@@ -4434,15 +4434,15 @@
       </c>
       <c r="L42" s="14"/>
       <c r="M42" s="55" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="56" t="s">
         <v>180</v>
       </c>
       <c r="B43" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C43" s="58" t="s">
         <v>181</v>
@@ -4475,15 +4475,15 @@
         <v>184</v>
       </c>
       <c r="M43" s="55" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>40</v>
@@ -4517,12 +4517,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>45</v>
@@ -4556,12 +4556,12 @@
       </c>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>55</v>
@@ -4595,12 +4595,12 @@
       </c>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>34</v>
@@ -4634,12 +4634,12 @@
       </c>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>37</v>
@@ -4673,12 +4673,12 @@
       </c>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>49</v>
@@ -4712,12 +4712,12 @@
       </c>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>52</v>
@@ -4751,12 +4751,12 @@
       </c>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>29</v>
@@ -4790,12 +4790,12 @@
       </c>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>116</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>117</v>
@@ -4829,12 +4829,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>112</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>113</v>
@@ -4868,12 +4868,12 @@
       </c>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>110</v>
@@ -4905,12 +4905,12 @@
       <c r="L54" s="11"/>
       <c r="M54" s="5"/>
     </row>
-    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="27" t="s">
         <v>106</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C55" s="22" t="s">
         <v>107</v>
@@ -4942,12 +4942,12 @@
       <c r="L55" s="11"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C56" s="36" t="s">
         <v>131</v>
@@ -4974,21 +4974,21 @@
         <v>19</v>
       </c>
       <c r="K56" s="70" t="s">
+        <v>501</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="M56" s="78" t="s">
         <v>502</v>
       </c>
-      <c r="L56" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="M56" s="78" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="56" t="s">
         <v>130</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C57" s="58" t="s">
         <v>131</v>
@@ -5021,22 +5021,22 @@
         <v>134</v>
       </c>
       <c r="M57" s="55" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="36" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C58" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>394</v>
-      </c>
       <c r="E58" s="13" t="s">
         <v>10</v>
       </c>
@@ -5056,19 +5056,19 @@
         <v>19</v>
       </c>
       <c r="K58" s="70" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L58" s="13"/>
       <c r="M58" s="80" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
         <v>269</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C59" s="22" t="s">
         <v>270</v>
@@ -5100,12 +5100,12 @@
       <c r="L59" s="11"/>
       <c r="M59" s="5"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
         <v>286</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>287</v>
@@ -5139,12 +5139,12 @@
       </c>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
         <v>126</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>127</v>
@@ -5177,12 +5177,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
         <v>168</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>169</v>
@@ -5216,12 +5216,12 @@
       </c>
       <c r="M62"/>
     </row>
-    <row r="63" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
         <v>214</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>215</v>
@@ -5257,12 +5257,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="27" t="s">
         <v>265</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>266</v>
@@ -5298,12 +5298,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
         <v>325</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>326</v>
@@ -5339,18 +5339,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="36" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C66" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>391</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>392</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>10</v>
@@ -5373,12 +5373,12 @@
       <c r="K66" s="12"/>
       <c r="L66" s="13"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C67" s="22" t="s">
         <v>89</v>
@@ -5410,12 +5410,12 @@
       <c r="L67" s="16"/>
       <c r="M67" s="2"/>
     </row>
-    <row r="68" spans="1:13" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="56" t="s">
         <v>318</v>
       </c>
       <c r="B68" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C68" s="58" t="s">
         <v>319</v>
@@ -5446,15 +5446,15 @@
       </c>
       <c r="L68" s="11"/>
       <c r="M68" s="86" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>124</v>
@@ -5487,12 +5487,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
         <v>219</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>220</v>
@@ -5519,21 +5519,21 @@
         <v>63</v>
       </c>
       <c r="K70" s="70" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L70" s="13" t="s">
         <v>64</v>
       </c>
       <c r="M70" s="77" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="27" t="s">
         <v>206</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>207</v>
@@ -5567,12 +5567,12 @@
       </c>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="27" t="s">
         <v>156</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C72" s="22" t="s">
         <v>157</v>
@@ -5599,27 +5599,27 @@
         <v>63</v>
       </c>
       <c r="K72" s="70" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L72" s="13" t="s">
         <v>160</v>
       </c>
       <c r="M72" s="77" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="56" t="s">
         <v>156</v>
       </c>
       <c r="B73" s="57" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C73" s="71" t="s">
         <v>157</v>
       </c>
       <c r="D73" s="64" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E73" s="60" t="s">
         <v>10</v>
@@ -5640,19 +5640,19 @@
         <v>19</v>
       </c>
       <c r="K73" s="59" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L73" s="60"/>
       <c r="M73" s="55" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="27" t="s">
         <v>152</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C74" s="22" t="s">
         <v>153</v>
@@ -5685,12 +5685,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="56" t="s">
         <v>306</v>
       </c>
       <c r="B75" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C75" s="58" t="s">
         <v>307</v>
@@ -5721,21 +5721,21 @@
       </c>
       <c r="L75" s="11"/>
       <c r="M75" s="55" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
         <v>73</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>74</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>10</v>
@@ -5765,12 +5765,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C77" s="22" t="s">
         <v>69</v>
@@ -5804,12 +5804,12 @@
       </c>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="27" t="s">
         <v>329</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C78" s="22" t="s">
         <v>330</v>
@@ -5842,12 +5842,12 @@
         <v>332</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="27" t="s">
         <v>60</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C79" s="22" t="s">
         <v>61</v>
@@ -5881,18 +5881,18 @@
       </c>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C80" s="22" t="s">
         <v>92</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>27</v>
@@ -5922,18 +5922,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="27" t="s">
         <v>100</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C81" s="22" t="s">
         <v>101</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>27</v>
@@ -5963,12 +5963,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
         <v>235</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C82" s="22" t="s">
         <v>236</v>
@@ -6004,12 +6004,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="27" t="s">
         <v>238</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C83" s="22" t="s">
         <v>239</v>
@@ -6045,12 +6045,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="56" t="s">
         <v>310</v>
       </c>
       <c r="B84" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C84" s="58" t="s">
         <v>311</v>
@@ -6083,21 +6083,21 @@
         <v>314</v>
       </c>
       <c r="M84" s="55" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="54" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B85" s="65" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C85" s="65" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D85" s="83" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E85" s="66" t="s">
         <v>10</v>
@@ -6106,7 +6106,7 @@
         <v>11</v>
       </c>
       <c r="G85" s="67" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H85" s="67" t="b">
         <v>1</v>
@@ -6120,18 +6120,18 @@
       <c r="K85" s="50"/>
       <c r="L85" s="14"/>
       <c r="M85" s="55" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="36" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C86" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D86" s="81" t="s">
         <v>367</v>
@@ -6143,7 +6143,7 @@
         <v>11</v>
       </c>
       <c r="G86" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H86" s="31" t="b">
         <v>1</v>
@@ -6157,12 +6157,12 @@
       <c r="K86" s="30"/>
       <c r="L86" s="14"/>
     </row>
-    <row r="87" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="21" t="s">
         <v>272</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C87" s="21" t="s">
         <v>273</v>
@@ -6196,18 +6196,18 @@
       </c>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C88" s="36" t="s">
+        <v>401</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>402</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>403</v>
       </c>
       <c r="E88" s="13" t="s">
         <v>10</v>
@@ -6232,18 +6232,18 @@
       </c>
       <c r="L88" s="13"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C89" s="36" t="s">
+        <v>397</v>
+      </c>
+      <c r="D89" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>399</v>
       </c>
       <c r="E89" s="13" t="s">
         <v>10</v>
@@ -6268,12 +6268,12 @@
       </c>
       <c r="L89" s="13"/>
     </row>
-    <row r="90" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="27" t="s">
         <v>349</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C90" s="22" t="s">
         <v>350</v>
@@ -6309,12 +6309,12 @@
         <v>358</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="27" t="s">
         <v>353</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>351</v>
@@ -6350,15 +6350,15 @@
         <v>358</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="5" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="5" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="39" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C92" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D92" s="36" t="s">
         <v>368</v>
@@ -6370,7 +6370,7 @@
         <v>11</v>
       </c>
       <c r="G92" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H92" s="31" t="b">
         <v>1</v>
@@ -6382,17 +6382,17 @@
         <v>19</v>
       </c>
       <c r="K92" s="34" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L92" s="14"/>
       <c r="M92"/>
     </row>
-    <row r="93" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="48" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B93" s="48" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C93" s="51" t="s">
         <v>352</v>
@@ -6428,15 +6428,15 @@
         <v>358</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="36" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D94" s="37" t="s">
         <v>221</v>
@@ -6448,7 +6448,7 @@
         <v>11</v>
       </c>
       <c r="G94" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H94" s="31" t="b">
         <v>1</v>
@@ -6460,22 +6460,22 @@
         <v>19</v>
       </c>
       <c r="K94" s="72" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L94" s="14"/>
       <c r="M94" s="55" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="36" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D95" s="37" t="s">
         <v>369</v>
@@ -6487,7 +6487,7 @@
         <v>11</v>
       </c>
       <c r="G95" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H95" s="31" t="b">
         <v>1</v>
@@ -6499,22 +6499,22 @@
         <v>19</v>
       </c>
       <c r="K95" s="61" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="L95" s="14"/>
       <c r="M95" s="80" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C96" s="35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D96" s="37" t="s">
         <v>370</v>
@@ -6526,7 +6526,7 @@
         <v>11</v>
       </c>
       <c r="G96" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H96" s="31" t="b">
         <v>1</v>
@@ -6538,28 +6538,28 @@
         <v>19</v>
       </c>
       <c r="K96" s="61" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="L96" s="62" t="s">
         <v>32</v>
       </c>
       <c r="M96" s="55" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="B97" s="48" t="s">
+        <v>412</v>
+      </c>
+      <c r="C97" s="49" t="s">
+        <v>434</v>
+      </c>
+      <c r="D97" s="82" t="s">
         <v>453</v>
       </c>
-      <c r="B97" s="48" t="s">
-        <v>413</v>
-      </c>
-      <c r="C97" s="49" t="s">
-        <v>435</v>
-      </c>
-      <c r="D97" s="82" t="s">
-        <v>454</v>
-      </c>
       <c r="E97" s="42" t="s">
         <v>10</v>
       </c>
@@ -6567,7 +6567,7 @@
         <v>11</v>
       </c>
       <c r="G97" s="44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H97" s="44" t="b">
         <v>1</v>
@@ -6581,15 +6581,15 @@
       <c r="K97" s="30"/>
       <c r="L97" s="14"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="36" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C98" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D98" s="37" t="s">
         <v>371</v>
@@ -6601,7 +6601,7 @@
         <v>11</v>
       </c>
       <c r="G98" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H98" s="31" t="b">
         <v>1</v>
@@ -6613,19 +6613,19 @@
         <v>19</v>
       </c>
       <c r="K98" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L98" s="14"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="36" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C99" s="35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D99" s="37" t="s">
         <v>372</v>
@@ -6637,7 +6637,7 @@
         <v>11</v>
       </c>
       <c r="G99" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H99" s="31" t="b">
         <v>1</v>
@@ -6649,19 +6649,19 @@
         <v>19</v>
       </c>
       <c r="K99" s="34" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L99" s="14"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="36" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D100" s="37" t="s">
         <v>373</v>
@@ -6673,7 +6673,7 @@
         <v>11</v>
       </c>
       <c r="G100" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H100" s="31" t="b">
         <v>1</v>
@@ -6685,16 +6685,16 @@
         <v>19</v>
       </c>
       <c r="K100" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L100" s="14"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>22</v>
@@ -6727,12 +6727,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C102" s="21" t="s">
         <v>84</v>
@@ -6768,15 +6768,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D103" s="24" t="s">
         <v>9</v>
@@ -6807,15 +6807,15 @@
       </c>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="36" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D104" s="37" t="s">
         <v>374</v>
@@ -6827,7 +6827,7 @@
         <v>11</v>
       </c>
       <c r="G104" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H104" s="31" t="b">
         <v>1</v>
@@ -6839,22 +6839,22 @@
         <v>19</v>
       </c>
       <c r="K104" s="30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L104" s="14"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C105" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>406</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>407</v>
       </c>
       <c r="E105" s="13" t="s">
         <v>10</v>
@@ -6879,18 +6879,18 @@
       </c>
       <c r="L105" s="13"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C106" s="36" t="s">
+        <v>403</v>
+      </c>
+      <c r="D106" s="14" t="s">
         <v>404</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>405</v>
       </c>
       <c r="E106" s="13" t="s">
         <v>10</v>
@@ -6915,12 +6915,12 @@
       </c>
       <c r="L106" s="13"/>
     </row>
-    <row r="107" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B107" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C107" s="21" t="s">
         <v>17</v>
@@ -6954,18 +6954,18 @@
         <v>347</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="28" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C108" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="D108" s="14" t="s">
         <v>400</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>401</v>
       </c>
       <c r="E108" s="13" t="s">
         <v>10</v>
@@ -6990,12 +6990,12 @@
       </c>
       <c r="L108" s="13"/>
     </row>
-    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="54" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C109" s="22" t="s">
         <v>344</v>
@@ -7028,21 +7028,21 @@
         <v>99</v>
       </c>
       <c r="M109" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="18" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C110" s="36" t="s">
+        <v>407</v>
+      </c>
+      <c r="D110" s="14" t="s">
         <v>408</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>409</v>
       </c>
       <c r="E110" s="13" t="s">
         <v>10</v>
@@ -7067,18 +7067,18 @@
       </c>
       <c r="L110" s="13"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="36" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C111" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="D111" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>390</v>
       </c>
       <c r="E111" s="13" t="s">
         <v>10</v>
@@ -7101,19 +7101,19 @@
       <c r="K111" s="12"/>
       <c r="L111" s="13"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="36" t="s">
+        <v>459</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="D112" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="B112" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="D112" s="36" t="s">
-        <v>461</v>
-      </c>
       <c r="E112" s="14" t="s">
         <v>10</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>11</v>
       </c>
       <c r="G112" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H112" s="31" t="b">
         <v>1</v>
@@ -7133,19 +7133,19 @@
         <v>19</v>
       </c>
       <c r="K112" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L112" s="14"/>
     </row>
-    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C113" s="22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>333</v>
@@ -7172,15 +7172,15 @@
         <v>334</v>
       </c>
       <c r="L113" s="14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114" s="21" t="s">
         <v>341</v>
       </c>
       <c r="B114" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C114" s="21" t="s">
         <v>342</v>
@@ -7214,12 +7214,12 @@
         <v>343</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="23" t="s">
         <v>339</v>
       </c>
       <c r="B115" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C115" s="23" t="s">
         <v>340</v>
@@ -7255,18 +7255,18 @@
         <v>338</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="18" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B116" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C116" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>397</v>
       </c>
       <c r="E116" s="13" t="s">
         <v>10</v>
@@ -7291,12 +7291,12 @@
       </c>
       <c r="L116" s="13"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="27" t="s">
         <v>315</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C117" s="22" t="s">
         <v>316</v>
@@ -7328,18 +7328,18 @@
       <c r="L117" s="11"/>
       <c r="M117" s="5"/>
     </row>
-    <row r="118" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="56" t="s">
         <v>252</v>
       </c>
       <c r="B118" s="57" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C118" s="71" t="s">
         <v>253</v>
       </c>
       <c r="D118" s="64" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E118" s="60" t="s">
         <v>10</v>
@@ -7364,15 +7364,15 @@
       </c>
       <c r="L118" s="52"/>
       <c r="M118" s="55" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="56" t="s">
         <v>252</v>
       </c>
       <c r="B119" s="57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C119" s="58" t="s">
         <v>253</v>
@@ -7405,15 +7405,15 @@
         <v>255</v>
       </c>
       <c r="M119" s="55" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="27" t="s">
         <v>289</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C120" s="22" t="s">
         <v>290</v>
@@ -7447,12 +7447,12 @@
       </c>
       <c r="M120" s="2"/>
     </row>
-    <row r="121" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="27" t="s">
         <v>296</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C121" s="22" t="s">
         <v>297</v>
@@ -7486,12 +7486,12 @@
       </c>
       <c r="M121" s="2"/>
     </row>
-    <row r="122" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="27" t="s">
         <v>293</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C122" s="22" t="s">
         <v>294</v>
@@ -7525,12 +7525,12 @@
       </c>
       <c r="M122" s="2"/>
     </row>
-    <row r="123" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" s="27" t="s">
         <v>300</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C123" s="22" t="s">
         <v>301</v>
@@ -7563,12 +7563,12 @@
         <v>299</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="27" t="s">
         <v>95</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C124" s="22" t="s">
         <v>96</v>
@@ -7601,12 +7601,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="27" t="s">
         <v>283</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C125" s="22" t="s">
         <v>284</v>
@@ -7639,12 +7639,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="27" t="s">
         <v>145</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C126" s="22" t="s">
         <v>146</v>
@@ -7677,12 +7677,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="27" t="s">
         <v>321</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C127" s="22" t="s">
         <v>322</v>
@@ -7715,12 +7715,12 @@
         <v>324</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="21" t="s">
         <v>210</v>
       </c>
       <c r="B128" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C128" s="21" t="s">
         <v>211</v>
@@ -7753,12 +7753,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="s">
         <v>259</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C129" s="21" t="s">
         <v>260</v>
@@ -7791,15 +7791,15 @@
         <v>213</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>359</v>
@@ -7812,15 +7812,15 @@
       <c r="J130" s="16"/>
       <c r="K130" s="30"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D131" s="35" t="s">
         <v>375</v>
@@ -7832,7 +7832,7 @@
         <v>11</v>
       </c>
       <c r="G131" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H131" s="31" t="b">
         <v>1</v>
@@ -7844,7 +7844,7 @@
         <v>19</v>
       </c>
       <c r="K131" s="32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>